<commit_message>
added descriptions and fixed chart
</commit_message>
<xml_diff>
--- a/quantum_graphs.xlsx
+++ b/quantum_graphs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="291" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="146" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,21 +15,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+  <si>
+    <t>Round Robin Algorithm</t>
+  </si>
   <si>
     <t>Quantum</t>
   </si>
   <si>
-    <t>RR Avg Waiting Time</t>
+    <t>Avg Waiting Time</t>
   </si>
   <si>
-    <t>Hybrid Avg Waiting Time</t>
+    <t>Avg Weighted Waiting</t>
   </si>
   <si>
-    <t>RR Weighted Waiting Time</t>
+    <t>Avg Response Time</t>
   </si>
   <si>
-    <t>Hybrid Weighted Waiting Time</t>
+    <t>Avg Weighted Response</t>
+  </si>
+  <si>
+    <t>Hybrid Algorithm</t>
   </si>
 </sst>
 </file>
@@ -39,11 +45,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -62,6 +69,11 @@
     </font>
     <font>
       <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -113,8 +125,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -190,7 +206,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -207,7 +223,7 @@
               <a:rPr sz="1300">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Scheduling Efficiency as Quantum Increases</a:t>
+              <a:t>Round Robin</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -216,19 +232,19 @@
     </c:title>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RR Avg Waiting Time</c:v>
+                  <c:v>Avg Waiting Time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -237,15 +253,23 @@
             <a:solidFill>
               <a:srgbClr val="004586"/>
             </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="13"/>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$8:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -282,71 +306,65 @@
                 <c:pt idx="11">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$14</c:f>
+              <c:f>Sheet1!$B$8:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>664.1</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>614.56</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>707.98</c:v>
+                  <c:v>614.24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>735.46</c:v>
+                  <c:v>598.12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>787.04</c:v>
+                  <c:v>616.76</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>812.6</c:v>
+                  <c:v>603.94</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>843.14</c:v>
+                  <c:v>608.76</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>867.42</c:v>
+                  <c:v>606.68</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>890.4</c:v>
+                  <c:v>602.98</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>902.98</c:v>
+                  <c:v>583.52</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>922.38</c:v>
+                  <c:v>577.52</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>937.3</c:v>
+                  <c:v>576</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>957.86</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v/>
+                  <c:v>577.72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$C$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hybrid Avg Waiting Time</c:v>
+                  <c:v>Avg Weighted Waiting</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -355,15 +373,23 @@
             <a:solidFill>
               <a:srgbClr val="ff420e"/>
             </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="13"/>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$8:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -400,71 +426,65 @@
                 <c:pt idx="11">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$14</c:f>
+              <c:f>Sheet1!$C$8:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>538.72</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>624.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>576.17</c:v>
+                  <c:v>622.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>610.9</c:v>
+                  <c:v>611.36</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>646.72</c:v>
+                  <c:v>624.31</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>665.332</c:v>
+                  <c:v>613.1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>698.72</c:v>
+                  <c:v>618.72</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>712.12</c:v>
+                  <c:v>606.68</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>731.44</c:v>
+                  <c:v>609.33</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>737.33</c:v>
+                  <c:v>594.53</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>751.36</c:v>
+                  <c:v>584.51</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>760.946</c:v>
+                  <c:v>578.78</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>772.21</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v/>
+                  <c:v>578.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$D$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RR Weighted Waiting Time</c:v>
+                  <c:v>Avg Response Time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -473,15 +493,23 @@
             <a:solidFill>
               <a:srgbClr val="ffd320"/>
             </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="13"/>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$8:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -518,71 +546,65 @@
                 <c:pt idx="11">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$14</c:f>
+              <c:f>Sheet1!$D$8:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>672.61</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>22.08</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>713.36</c:v>
+                  <c:v>67.72</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>744.71</c:v>
+                  <c:v>110.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>791.21</c:v>
+                  <c:v>147.92</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>817.06</c:v>
+                  <c:v>184.94</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>846.77</c:v>
+                  <c:v>221.26</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>866.59</c:v>
+                  <c:v>252.46</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>892.38</c:v>
+                  <c:v>280.44</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>906.13</c:v>
+                  <c:v>307.72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>924.99</c:v>
+                  <c:v>330.1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>937.69</c:v>
+                  <c:v>349.52</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>958.51</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v/>
+                  <c:v>368.16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>Sheet1!$E$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hybrid Weighted Waiting Time</c:v>
+                  <c:v>Avg Weighted Response</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -591,15 +613,23 @@
             <a:solidFill>
               <a:srgbClr val="579d1c"/>
             </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="13"/>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$8:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -636,67 +666,60 @@
                 <c:pt idx="11">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$14</c:f>
+              <c:f>Sheet1!$E$8:$E$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>192.57</c:v>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>21.43</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>220.26</c:v>
+                  <c:v>65.97</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>241.69</c:v>
+                  <c:v>107.47</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>265.28</c:v>
+                  <c:v>144.22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>273.34</c:v>
+                  <c:v>180.31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>297.78</c:v>
+                  <c:v>215.74</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>303.82</c:v>
+                  <c:v>246.06</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>315.55</c:v>
+                  <c:v>273.18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>315.5</c:v>
+                  <c:v>299.66</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>326.04</c:v>
+                  <c:v>321.33</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>331.4</c:v>
+                  <c:v>340.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>338.39</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v/>
+                  <c:v>358.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
         </c:ser>
-        <c:gapWidth val="100"/>
-        <c:axId val="30488777"/>
-        <c:axId val="57155213"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="30488777"/>
+        <c:axId val="81676232"/>
+        <c:axId val="7855058"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="81676232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -732,14 +755,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="57155213"/>
+        <c:crossAx val="7855058"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="57155213"/>
+        <c:axId val="7855058"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +787,7 @@
                   <a:rPr sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Time Steps</a:t>
+                  <a:t>CPU Time</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -784,7 +804,640 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="30488777"/>
+        <c:crossAx val="81676232"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Hybrid</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg Waiting Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$23:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$23:$B$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>536.38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>537.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>530.78</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>552.28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>554.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>552.24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>551.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>567.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>564</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>562.72</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>548</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>560.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg Weighted Waiting</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$23:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$23:$C$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>395.72</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>396.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>398.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>425.16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>436.89</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>443.71</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>440.63</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>460.56</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>471.72</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>473.21</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>449.36</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>463.04</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg Response Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$23:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$23:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>202.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>241.14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>246.16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>262.02</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>269.72</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>274.04</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>281.14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>299.78</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>306.64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>306.88</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>316.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg Weighted Response</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:smooth val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$23:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$23:$E$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>88.76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>123.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>129.94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>144.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>153.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>161.67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>168.58</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>180.98</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>189.63</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>197.35</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>197.97</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>206.45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="342804"/>
+        <c:axId val="6048539"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="342804"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Quantum</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="6048539"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="6048539"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>CPU Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="342804"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -823,16 +1476,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>639000</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>83880</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>273600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1224720</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>343800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -840,12 +1493,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="639000" y="2522160"/>
+        <a:off x="6234840" y="160200"/>
         <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>293400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>26640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>363600</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>15120</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="6254640" y="3440160"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -859,244 +1542,485 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A6:E34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
+      <selection pane="topLeft" activeCell="D44" activeCellId="0" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6887755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9336734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1581632653061"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B7" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="C7" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>664.1</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>538.72</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>672.61</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>192.57</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>707.98</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>576.17</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>713.36</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>220.26</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>735.46</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>610.9</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>744.71</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>241.69</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>787.04</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>646.72</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>791.21</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>265.28</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>812.6</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>665.332</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>817.06</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>273.34</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>843.14</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>698.72</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>846.77</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>297.78</v>
+      <c r="E7" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>867.42</v>
+        <v>614.56</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>712.12</v>
+        <v>624.6</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>866.59</v>
+        <v>22.08</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>303.82</v>
+        <v>21.43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>890.4</v>
+        <v>614.24</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>731.44</v>
+        <v>622.25</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>892.38</v>
+        <v>67.72</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>315.55</v>
+        <v>65.97</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>902.98</v>
+        <v>598.12</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>737.33</v>
+        <v>611.36</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>906.13</v>
+        <v>110.2</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>315.5</v>
+        <v>107.47</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>922.38</v>
+        <v>616.76</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>751.36</v>
+        <v>624.31</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>924.99</v>
+        <v>147.92</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>326.04</v>
+        <v>144.22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>937.3</v>
+        <v>603.94</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>760.946</v>
+        <v>613.1</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>937.69</v>
+        <v>184.94</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>331.4</v>
+        <v>180.31</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>608.76</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>618.72</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>221.26</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>215.74</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>606.68</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>606.68</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>252.46</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>246.06</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>602.98</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>609.33</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>280.44</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>273.18</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>583.52</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>594.53</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>307.72</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>299.66</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>577.52</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>584.51</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>330.1</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>321.33</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>576</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>578.78</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>349.52</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>340.1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B13" s="0" t="n">
-        <v>957.86</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>772.21</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>958.51</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>338.39</v>
+      <c r="B19" s="0" t="n">
+        <v>577.72</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>578.98</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>368.16</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>358.08</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>536.38</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>395.72</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>202.9</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>88.76</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>537.7</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>396.7</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>241.14</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>123.99</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>530.78</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>398.84</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>246.16</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>129.94</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>552.28</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>425.16</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>262.02</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>144.35</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>554.92</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>436.89</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>269.72</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>153.92</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>552.24</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>443.71</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>274.04</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>161.67</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>551.1</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>440.63</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>281.14</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>168.58</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>567.02</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>460.56</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>294</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>180.98</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>564</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>471.72</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>299.78</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>189.63</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>562.72</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>473.21</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>306.64</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>197.35</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>548</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>449.36</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>306.88</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>197.97</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>560.8</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>463.04</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>316.6</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>206.45</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B21:E21"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>